<commit_message>
Bài 29 - DataProvider - Data Driven Testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataCRM.xlsx
+++ b/src/test/resources/testdata/DataCRM.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_012025\SeleniumMavenTestNGParallel012025\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90D485D-CB8E-4D69-9B6D-EE933008668D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF08BE27-7CC2-45E1-B80F-FF7D661F0538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4536" yWindow="1800" windowWidth="22704" windowHeight="13872" xr2:uid="{16F407ED-D0A3-4422-9924-21C493E068E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{16F407ED-D0A3-4422-9924-21C493E068E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Customer" sheetId="2" r:id="rId2"/>
-    <sheet name="Project" sheetId="3" r:id="rId3"/>
+    <sheet name="Login_DataProvider" sheetId="4" r:id="rId2"/>
+    <sheet name="Customer" sheetId="2" r:id="rId3"/>
+    <sheet name="Project" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>EMAIL</t>
   </si>
@@ -80,13 +81,27 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>admin2@example.com</t>
+  </si>
+  <si>
+    <t>A12345</t>
+  </si>
+  <si>
+    <t>admin3@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -114,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,9 +151,6 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill/>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -153,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -161,18 +173,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,15 +512,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E15B5E-F78D-4B55-BCB7-5E4001C87BFB}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.15234375"/>
-    <col min="2" max="2" customWidth="true" width="14.4609375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.69140625"/>
+    <col min="1" max="1" width="23.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" customWidth="1"/>
+    <col min="3" max="3" width="13.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -538,10 +538,10 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>123456</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -549,10 +549,10 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>123</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -566,18 +566,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB25C49-D927-494D-BEC5-FA4EC6D6829F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.15234375" customWidth="1"/>
+    <col min="2" max="2" width="14.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{24A9BCE9-3066-434F-9E74-B0114C87AB7B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{F07A8249-63D3-4D27-864D-544A5D276239}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{2F0AAD4D-7198-46F3-9DD3-4732642E15FC}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{13CC10FE-3E10-4D6F-95C7-5A31749CE30D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89DD701-96A6-4F0A-9DAD-7BAD198FAA09}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.15234375"/>
-    <col min="3" max="3" customWidth="true" width="17.53515625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.15234375"/>
+    <col min="1" max="1" width="20.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.53515625" customWidth="1"/>
+    <col min="4" max="4" width="17.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,10 +661,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -616,7 +682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF39E1D-B4B2-42DB-96EC-47A504741F82}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>